<commit_message>
feat : stock and sales adjustments, adding dashboard
</commit_message>
<xml_diff>
--- a/public/template_penjualan.xlsx
+++ b/public/template_penjualan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D22985-8798-41FD-8E3A-F32601B0F661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A133E152-061A-4CEB-850A-75096B6B49E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,10 +417,10 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>